<commit_message>
Calculo de tabla de amortización de prestamo establew
</commit_message>
<xml_diff>
--- a/readme/Amortizaciones al vencimiento.xlsx
+++ b/readme/Amortizaciones al vencimiento.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\FIDEGARANTE\Cartera2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\laravel\finance\readme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B212C1C-F092-4C96-A3ED-376DBB00E656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940D82BA-70B2-4295-8B9E-3E230A3E0CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{166291DA-5AAD-E24E-9618-91DDFBF7AEBE}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{166291DA-5AAD-E24E-9618-91DDFBF7AEBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -470,7 +481,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -563,13 +574,17 @@
       <c r="D5" s="3">
         <v>0.24</v>
       </c>
+      <c r="G5">
+        <f>24/100</f>
+        <v>0.24</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -578,7 +593,7 @@
       </c>
       <c r="D7" s="2">
         <f ca="1">TODAY()</f>
-        <v>44396</v>
+        <v>45032</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -619,7 +634,7 @@
       </c>
       <c r="B11" s="2">
         <f ca="1">D7</f>
-        <v>44396</v>
+        <v>45032</v>
       </c>
       <c r="C11" s="6">
         <f>D1</f>
@@ -644,27 +659,31 @@
       </c>
       <c r="B12" s="2">
         <f ca="1">IF(A12=" "," ",IF(D$3="mensual",DATE(YEAR(B11),MONTH(B11)+1,DAY(D$4)),B11+14))</f>
-        <v>44410</v>
+        <v>45048</v>
       </c>
       <c r="C12" s="4">
         <f ca="1">IF(B12=" "," ",C11-E12)</f>
-        <v>100000</v>
+        <v>83333.333333333328</v>
       </c>
       <c r="E12" s="4">
         <f ca="1">IF(C12=" "," ",IF(D$6="Al vencimiento",IF(A12=D$2,C11,0),D$1/D$2))</f>
-        <v>0</v>
+        <v>16666.666666666668</v>
       </c>
       <c r="F12" s="4">
         <f ca="1">IF(E12=" "," ",C11*D$5/360*(B12-B11))</f>
-        <v>1200</v>
+        <v>1066.6666666666667</v>
       </c>
       <c r="G12" s="4">
         <f ca="1">IF(F12=" "," ",F12*I$2)</f>
-        <v>192</v>
+        <v>170.66666666666669</v>
       </c>
       <c r="H12" s="4">
         <f ca="1">IF(G12=" "," ",SUM(D12:F12))</f>
-        <v>1200</v>
+        <v>17733.333333333336</v>
+      </c>
+      <c r="J12">
+        <f ca="1">(B12-B11)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -674,152 +693,172 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13:B50" ca="1" si="0">IF(A13=" "," ",IF(D$3="mensual",DATE(YEAR(B12),MONTH(B12)+1,DAY(D$4)),B12+14))</f>
-        <v>44441</v>
+        <v>45079</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ref="C13:C50" ca="1" si="1">IF(B13=" "," ",C12-E13)</f>
-        <v>100000</v>
+        <v>66666.666666666657</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" ref="E13:E50" ca="1" si="2">IF(C13=" "," ",IF(D$6="Al vencimiento",IF(A13=D$2,C12,0),D$1/D$2))</f>
-        <v>0</v>
+        <v>16666.666666666668</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" ref="F13:F50" ca="1" si="3">IF(E13=" "," ",C12*D$5/360*(B13-B12))</f>
-        <v>2066.666666666667</v>
+        <v>1722.2222222222217</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" ref="G13:G50" ca="1" si="4">IF(F13=" "," ",F13*I$2)</f>
-        <v>330.66666666666674</v>
+        <v>275.55555555555549</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" ref="H13:H50" ca="1" si="5">IF(G13=" "," ",SUM(D13:F13))</f>
-        <v>2066.666666666667</v>
+        <v>18388.888888888891</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13:J17" ca="1" si="6">(B13-B12)</f>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" ref="A14:A50" si="6">IF(OR(A13=D$2,A13&gt;D$2)," ",A13+1)</f>
+        <f t="shared" ref="A14:A50" si="7">IF(OR(A13=D$2,A13&gt;D$2)," ",A13+1)</f>
         <v>3</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>44471</v>
+        <v>45109</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>100000</v>
+        <v>49999.999999999985</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>16666.666666666668</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>2000.0000000000002</v>
+        <v>1333.333333333333</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" ca="1" si="4"/>
-        <v>320.00000000000006</v>
+        <v>213.33333333333329</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>2000.0000000000002</v>
+        <v>18000</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ca="1" si="6"/>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>44502</v>
+        <v>45140</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>100000</v>
+        <v>33333.333333333314</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>16666.666666666668</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>2066.666666666667</v>
+        <v>1033.333333333333</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" ca="1" si="4"/>
-        <v>330.66666666666674</v>
+        <v>165.33333333333329</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>2066.666666666667</v>
+        <v>17700</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ca="1" si="6"/>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>44532</v>
+        <v>45171</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>100000</v>
+        <f ca="1">IF(B16=" "," ",C15-E16)</f>
+        <v>16666.666666666646</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>16666.666666666668</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>2000.0000000000002</v>
+        <v>688.88888888888857</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" ca="1" si="4"/>
-        <v>320.00000000000006</v>
+        <v>110.22222222222217</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>2000.0000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17355.555555555555</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ca="1" si="6"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>44563</v>
+        <v>45201</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f ca="1">IF(B17=" "," ",C16-E17)</f>
+        <v>-2.1827872842550278E-11</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>100000</v>
+        <f ca="1">IF(C17=" "," ",IF(D$6="Al vencimiento",IF(A17=D$2,C16,0),D$1/D$2))</f>
+        <v>16666.666666666668</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>2066.666666666667</v>
+        <v>333.33333333333292</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" ca="1" si="4"/>
-        <v>330.66666666666674</v>
+        <v>53.333333333333265</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>102066.66666666667</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17000</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="6"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B18" s="2" t="str">
@@ -847,9 +886,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B19" s="2" t="str">
@@ -877,9 +916,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B20" s="2" t="str">
@@ -907,9 +946,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B21" s="2" t="str">
@@ -937,9 +976,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B22" s="2" t="str">
@@ -967,9 +1006,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B23" s="2" t="str">
@@ -997,9 +1036,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B24" s="2" t="str">
@@ -1027,9 +1066,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B25" s="2" t="str">
@@ -1057,9 +1096,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B26" s="2" t="str">
@@ -1087,9 +1126,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B27" s="2" t="str">
@@ -1117,9 +1156,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B28" s="2" t="str">
@@ -1147,9 +1186,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B29" s="2" t="str">
@@ -1177,9 +1216,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B30" s="2" t="str">
@@ -1207,9 +1246,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B31" s="2" t="str">
@@ -1237,9 +1276,9 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B32" s="2" t="str">
@@ -1269,7 +1308,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B33" s="2" t="str">
@@ -1299,7 +1338,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B34" s="2" t="str">
@@ -1329,7 +1368,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B35" s="2" t="str">
@@ -1359,7 +1398,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B36" s="2" t="str">
@@ -1389,7 +1428,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B37" s="2" t="str">
@@ -1419,7 +1458,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B38" s="2" t="str">
@@ -1449,7 +1488,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B39" s="2" t="str">
@@ -1479,7 +1518,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B40" s="2" t="str">
@@ -1509,7 +1548,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B41" s="2" t="str">
@@ -1539,7 +1578,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B42" s="2" t="str">
@@ -1569,7 +1608,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B43" s="2" t="str">
@@ -1599,7 +1638,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B44" s="2" t="str">
@@ -1629,7 +1668,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B45" s="2" t="str">
@@ -1659,7 +1698,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B46" s="2" t="str">
@@ -1689,7 +1728,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B47" s="2" t="str">
@@ -1719,7 +1758,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B48" s="2" t="str">
@@ -1749,7 +1788,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B49" s="2" t="str">
@@ -1779,7 +1818,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B50" s="2" t="str">

</xml_diff>